<commit_message>
add the parkinson index
</commit_message>
<xml_diff>
--- a/deepface/Excel/Data.xlsx
+++ b/deepface/Excel/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>angry</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>neutral</t>
+  </si>
+  <si>
+    <t>Parkinson</t>
   </si>
 </sst>
 </file>
@@ -392,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,8 +423,11 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -446,8 +452,11 @@
       <c r="H2">
         <v>20.88617533445358</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -472,8 +481,11 @@
       <c r="H3">
         <v>14.34916406869888</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -497,6 +509,9 @@
       </c>
       <c r="H4">
         <v>2.00349036604166</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>